<commit_message>
added boolean last station to beacons
</commit_message>
<xml_diff>
--- a/resources/Green Line.xlsx
+++ b/resources/Green Line.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07de44e608f1ac43/Documents/GitHub/ECE1140-Project/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3521C211-4A3E-4F71-A8FB-F98946140EDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{761FD9F6-EA9D-4A3F-9685-CC3FB99ABCF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21345" yWindow="2535" windowWidth="19200" windowHeight="9750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="91">
   <si>
     <t>Block Number</t>
   </si>
@@ -260,46 +260,49 @@
     <t>B0</t>
   </si>
   <si>
-    <t>JERRY,TRUE,BOTH</t>
-  </si>
-  <si>
-    <t>EDGEBROOK,TRUE,LEFT</t>
-  </si>
-  <si>
-    <t>PIONEER,TRUE,LEFT</t>
-  </si>
-  <si>
-    <t>WHITED,TRUE,BOTH</t>
-  </si>
-  <si>
-    <t>SOUTH BANK,TRUE,LEFT</t>
-  </si>
-  <si>
-    <t>CENTRAL,TRUE,RIGHT</t>
-  </si>
-  <si>
-    <t>INGLEWOOD,TRUE,RIGHT</t>
-  </si>
-  <si>
-    <t>OVERBROOK,TRUE,RIGHT</t>
-  </si>
-  <si>
-    <t>GLENBURY,TRUE,RIGHT</t>
-  </si>
-  <si>
-    <t>DORMONT,TRUE,RIGHT</t>
-  </si>
-  <si>
-    <t>MT LEBANON,TRUE,BOTH</t>
-  </si>
-  <si>
-    <t>POPLAR,TRUE,LEFT</t>
-  </si>
-  <si>
-    <t>CASTLE SHANNON,TRUE,LEFT</t>
-  </si>
-  <si>
-    <t>INGLEWOOD,TRUE,LEFT</t>
+    <t>PIONEER,TRUE,LEFT,FALSE</t>
+  </si>
+  <si>
+    <t>EDGEBROOK,TRUE,LEFT,FALSE</t>
+  </si>
+  <si>
+    <t>JERRY,TRUE,BOTH,FALSE</t>
+  </si>
+  <si>
+    <t>WHITED,TRUE,BOTH,FALSE</t>
+  </si>
+  <si>
+    <t>SOUTH BANK,TRUE,LEFT,FALSE</t>
+  </si>
+  <si>
+    <t>CENTRAL,TRUE,RIGHT,FALSE</t>
+  </si>
+  <si>
+    <t>INGLEWOOD,TRUE,RIGHT,FALSE</t>
+  </si>
+  <si>
+    <t>GLENBURY,TRUE,RIGHT,FALSE</t>
+  </si>
+  <si>
+    <t>DORMONT,TRUE,RIGHT,FALSE</t>
+  </si>
+  <si>
+    <t>MT LEBANON,TRUE,BOTH,FALSE</t>
+  </si>
+  <si>
+    <t>OVERBROOK,TRUE,RIGHT,TRUE</t>
+  </si>
+  <si>
+    <t>POPLAR,TRUE,LEFT,FALSE</t>
+  </si>
+  <si>
+    <t>CASTLE SHANNON,TRUE,LEFT,FALSE</t>
+  </si>
+  <si>
+    <t>OVERBROOK,TRUE,RIGHT,FALSE</t>
+  </si>
+  <si>
+    <t>INGLEWOOD,TRUE,LEFT,FALSE</t>
   </si>
 </sst>
 </file>
@@ -739,8 +742,8 @@
   <dimension ref="A1:U151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G142" sqref="G142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -750,8 +753,8 @@
     <col min="3" max="3" width="8.453125" style="3" customWidth="1"/>
     <col min="4" max="4" width="17.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="3" customWidth="1"/>
     <col min="9" max="9" width="10.54296875" style="3" customWidth="1"/>
     <col min="10" max="11" width="13.26953125" style="3" customWidth="1"/>
@@ -840,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H2" s="3">
         <v>100</v>
@@ -925,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H4" s="3">
         <v>100</v>
@@ -1426,10 +1429,10 @@
         <v>2</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H17" s="3">
         <v>150</v>
@@ -1925,10 +1928,9 @@
       <c r="E30" s="3">
         <v>1</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G30" s="11"/>
       <c r="H30" s="3">
         <v>50</v>
       </c>
@@ -3054,7 +3056,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G58" s="8"/>
       <c r="H58" s="3">
@@ -3378,7 +3380,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H66" s="3">
         <v>200</v>
@@ -3679,7 +3681,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H74" s="3">
         <v>100</v>
@@ -3836,10 +3838,10 @@
         <v>2</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H78" s="3">
         <v>300</v>
@@ -4905,7 +4907,7 @@
         <v>0</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H106" s="3">
         <v>100</v>
@@ -5242,7 +5244,7 @@
         <v>0</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H115" s="3">
         <f>100+62</f>
@@ -5583,7 +5585,7 @@
         <v>0</v>
       </c>
       <c r="F124" s="8" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="G124" s="8"/>
       <c r="H124" s="3">
@@ -5950,7 +5952,7 @@
         <v>0</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G133" s="8"/>
       <c r="H133" s="3">

</xml_diff>